<commit_message>
Prueba exitosa de TidyR
</commit_message>
<xml_diff>
--- a/datos/empleo_genero.xlsx
+++ b/datos/empleo_genero.xlsx
@@ -1106,16 +1106,16 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AZ461"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="S439" sqref="S439"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" hidden="1" customWidth="1"/>
-    <col min="4" max="15" width="18.42578125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="15" width="18.42578125" customWidth="1"/>
     <col min="16" max="27" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="21" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="18.42578125" bestFit="1" customWidth="1"/>

</xml_diff>